<commit_message>
Pom Implementation and testNG implementation done Added a method convertDynamicXpathToWebElement() in WebDriverUtility Instantiated all pom pages in BaseClass
</commit_message>
<xml_diff>
--- a/src/test/resources/VtigerCRMTestData.xlsx
+++ b/src/test/resources/VtigerCRMTestData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\VtigerCRMHASA9\src\test\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2DF9B6B5-5E0C-464B-BCF3-BF2A2EFFC2F2}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1D60C1F9-9FD4-4256-B688-3582B276845D}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="19488" windowHeight="3996" activeTab="3" xr2:uid="{A6492B4B-4497-484C-9067-5A512381FFD5}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="42">
   <si>
     <t>TestCase Name</t>
   </si>
@@ -141,9 +141,6 @@
     <t>2025-10-18</t>
   </si>
   <si>
-    <t>Due date</t>
-  </si>
-  <si>
     <t>2025-11-26</t>
   </si>
   <si>
@@ -151,6 +148,12 @@
   </si>
   <si>
     <t>Events</t>
+  </si>
+  <si>
+    <t>Due Date</t>
+  </si>
+  <si>
+    <t>Fail</t>
   </si>
 </sst>
 </file>
@@ -838,7 +841,7 @@
         <v>10</v>
       </c>
       <c r="E5" t="s">
-        <v>19</v>
+        <v>41</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.3">
@@ -1117,7 +1120,9 @@
       <c r="D6" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="E6" s="1"/>
+      <c r="E6" t="s">
+        <v>19</v>
+      </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7" s="1"/>
@@ -1177,7 +1182,7 @@
   <dimension ref="A1:E6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1214,12 +1219,14 @@
         <v>32</v>
       </c>
       <c r="C2" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="D2" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="D2" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="E2" s="1"/>
+      <c r="E2" t="s">
+        <v>19</v>
+      </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" s="1"/>
@@ -1249,10 +1256,10 @@
       <c r="A5" s="1"/>
       <c r="B5" s="8"/>
       <c r="C5" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="D5" s="1" t="s">
         <v>37</v>
-      </c>
-      <c r="D5" s="1" t="s">
-        <v>38</v>
       </c>
       <c r="E5" s="1"/>
     </row>

</xml_diff>